<commit_message>
Renamed ICustomExcelReading to ICustomExcelRowReading
</commit_message>
<xml_diff>
--- a/data/Artifact.xlsx
+++ b/data/Artifact.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\GenshinSim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB29983-1D0B-4EA8-8FFA-CC6EEE587782}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB2F55E-846A-414A-ABC1-6461CAE88964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ArtifactSetDataTable" sheetId="1" r:id="rId1"/>
@@ -51,13 +51,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>,
-[StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
-,
-[StatisticBoost,Stackable;Attack_Percentage=0.09,MaxNumStacks=0,InitialNumStacks=0;,StatisticBoost,Triggerable;DamageModifier_PhysicalDamage=0.25;],</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Bloodstained Chivalry</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -66,6 +59,13 @@
 [StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
 ,
 [StatisticBoost,Triggerable;DamageModifier_ChargedAttack=0.25;],</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>,
+[StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
+,
+[StatisticBoost,Stackable;Attack_Percentage=0.09,MaxNumStacks=2,InitialNumStacks=0;,StatisticBoost,Triggerable;DamageModifier_PhysicalDamage=0.25;],</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -400,7 +400,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -435,15 +435,15 @@
         <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Made use of merged column reading
</commit_message>
<xml_diff>
--- a/data/Artifact.xlsx
+++ b/data/Artifact.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Workspace\GenshinSim\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB2F55E-846A-414A-ABC1-6461CAE88964}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B23E6ED-F659-4A0A-90E8-CAB85C86460A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>### FIELD_NAME</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -55,18 +55,16 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>,
-[StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
-,
-[StatisticBoost,Triggerable;DamageModifier_ChargedAttack=0.25;],</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>,
-[StatisticBoost;DamageModifier_PhysicalDamage=0.25;],
-,
-[StatisticBoost,Stackable;Attack_Percentage=0.09,MaxNumStacks=2,InitialNumStacks=0;,StatisticBoost,Triggerable;DamageModifier_PhysicalDamage=0.25;],</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+    <t>StatisticBoost;DamageModifier_PhysicalDamage=0.25;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StatisticBoost,Stackable;Attack_Percentage=0.09,MaxNumStacks=2,InitialNumStacks=0;,
+StatisticBoost,Triggerable;DamageModifier_PhysicalDamage=0.25;</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StatisticBoost,Triggerable;DamageModifier_ChargedAttack=0.25;</t>
   </si>
 </sst>
 </file>
@@ -109,13 +107,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -397,21 +404,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="15.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="26.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="135.5" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="9" style="1"/>
+    <col min="3" max="7" width="76.375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -419,34 +426,49 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>2</v>
       </c>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="2"/>
+      <c r="D3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="2"/>
+      <c r="D4" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:G2"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>